<commit_message>
kept a single scenario for every triptype to run on jenkins
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/Air/Air_Amadeus.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/Air/Air_Amadeus.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="37">
   <si>
     <t>Description</t>
   </si>
@@ -72,9 +72,6 @@
     <t>AmadeusWS air oneway booking for DOMESTIC location for 1 Adult with Login</t>
   </si>
   <si>
-    <t>Search|AddToCart|CHECKOUTTRIP|LOGIN|ENTERPAXINFO|CONFIRMPAXINFO|PAYNOW</t>
-  </si>
-  <si>
     <t>OneWay</t>
   </si>
   <si>
@@ -96,27 +93,9 @@
     <t>Registered</t>
   </si>
   <si>
-    <t>AmadeusWS air oneway booking for DOMESTIC location for 1 Adult and 1 child with Login.</t>
-  </si>
-  <si>
     <t>JFK-LAS</t>
   </si>
   <si>
-    <t>AmadeusWS air oneway booking for DOMESTIC location for 1 adult and 1 infant with Login.</t>
-  </si>
-  <si>
-    <t>AmadeusWS air oneway booking for DOMESTIC location for 1 adult . 1 child and 1 infant with Login.</t>
-  </si>
-  <si>
-    <t>Search|SETFILTERS|AddToCart</t>
-  </si>
-  <si>
-    <t>airlines</t>
-  </si>
-  <si>
-    <t>AA/NK</t>
-  </si>
-  <si>
     <t>AmadeusWS air round trip booking for DOMESTIC location for 1 adult with Login.</t>
   </si>
   <si>
@@ -132,27 +111,6 @@
     <t>20-30</t>
   </si>
   <si>
-    <t>AmadeusWS air round trip booking for DOMESTIC location for 1 adult and 1 child with Login.</t>
-  </si>
-  <si>
-    <t>stop|cabin</t>
-  </si>
-  <si>
-    <t>one|business</t>
-  </si>
-  <si>
-    <t>AmadeusWS air round trip booking for DOMESTIC location for 1 adult and 1 infant with Login.</t>
-  </si>
-  <si>
-    <t>Search|AddToCart|CHECKOUTTRIP|LOGIN</t>
-  </si>
-  <si>
-    <t>AmadeusWS air round trip booking for DOMESTIC location for 1 adult. 1 child and 1 infant with Login.</t>
-  </si>
-  <si>
-    <t>DFW-LAS</t>
-  </si>
-  <si>
     <t>AmadeusWS air MULTICITY booking for DOMESTIC location for 1 Adult with Login.</t>
   </si>
   <si>
@@ -165,46 +123,7 @@
     <t>53|64|71</t>
   </si>
   <si>
-    <t>AmadeusWS air MULTICITY booking for DOMESTIC location 1 Adult and 1 child with Login.</t>
-  </si>
-  <si>
     <t>Search|AddToCart|CHECKOUTTRIP|LOGIN|ENTERPAXINFO|CONFIRMPAXINFO</t>
-  </si>
-  <si>
-    <t>AmadeusWS air MULTICITY booking for DOMESTIC location for 1 adult and 1 infant with Login.</t>
-  </si>
-  <si>
-    <t>AmadeusWS air MULTICITY booking for DOMESTIC location for 1 adult .1 child and 1 infant with Login.</t>
-  </si>
-  <si>
-    <t>AmadeusWS air oneway booking for INTERNATIONAL location for 1 Adult with Login.</t>
-  </si>
-  <si>
-    <t>JFK-PAR</t>
-  </si>
-  <si>
-    <t>AmadeusWS air oneway booking for INTERNATIONAL location 1 Adult and 1 child with Login.</t>
-  </si>
-  <si>
-    <t>AmadeusWS air oneway booking for INTERNATIONAL location for 1 adult and 1 infant with Login.</t>
-  </si>
-  <si>
-    <t>AmadeusWS air oneway booking for INTERNATIONAL location for 1 adult. 1 child and 1 infant with Login.</t>
-  </si>
-  <si>
-    <t>AmadeusWS air round trip booking for INTERNATIONAL location for 1 Adult with Login.</t>
-  </si>
-  <si>
-    <t>AmadeusWS air MULTICITY booking for INTERNATIONAL location for 1 Adult with Login.</t>
-  </si>
-  <si>
-    <t>SIN-BKK|BKK-SIN|SIN-HKG</t>
-  </si>
-  <si>
-    <t>12|20|22</t>
-  </si>
-  <si>
-    <t>Guest</t>
   </si>
   <si>
     <t>RoviaBucks</t>
@@ -214,7 +133,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,18 +153,6 @@
       <sz val="10"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -268,7 +175,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -312,17 +219,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -382,19 +278,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -424,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -433,10 +316,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -448,60 +334,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="50">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -1055,25 +936,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1479,8 +1341,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q9" totalsRowShown="0" headerRowDxfId="49" headerRowBorderDxfId="48">
-  <autoFilter ref="A1:Q9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="49" headerRowBorderDxfId="48">
+  <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
     <tableColumn id="1" name="Description" dataDxfId="47"/>
     <tableColumn id="2" name="ExecutionPipeline" dataDxfId="46"/>
@@ -1505,52 +1367,52 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:Q6" totalsRowShown="0">
-  <autoFilter ref="A1:Q6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:Q2" totalsRowShown="0">
+  <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
     <tableColumn id="1" name="Description" dataDxfId="30"/>
-    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="29"/>
-    <tableColumn id="3" name="TripType" dataDxfId="28"/>
-    <tableColumn id="4" name="AirPortPairs" dataDxfId="27"/>
-    <tableColumn id="5" name="TravelDates" dataDxfId="26"/>
+    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="0"/>
+    <tableColumn id="3" name="TripType" dataDxfId="29"/>
+    <tableColumn id="4" name="AirPortPairs" dataDxfId="28"/>
+    <tableColumn id="5" name="TravelDates" dataDxfId="27"/>
     <tableColumn id="6" name="Adults"/>
     <tableColumn id="7" name="Infants"/>
     <tableColumn id="8" name="Children"/>
-    <tableColumn id="9" name="IncludeNearByAirPorts" dataDxfId="25"/>
-    <tableColumn id="10" name="CabinType" dataDxfId="24"/>
-    <tableColumn id="11" name="NonStopFlight" dataDxfId="23"/>
+    <tableColumn id="9" name="IncludeNearByAirPorts" dataDxfId="26"/>
+    <tableColumn id="10" name="CabinType" dataDxfId="25"/>
+    <tableColumn id="11" name="NonStopFlight" dataDxfId="24"/>
     <tableColumn id="12" name="AirLines"/>
-    <tableColumn id="13" name="PaymentMode" dataDxfId="22"/>
-    <tableColumn id="14" name="Supplier" dataDxfId="21"/>
-    <tableColumn id="15" name="UserType" dataDxfId="20"/>
-    <tableColumn id="16" name="PostFilters" dataDxfId="19"/>
-    <tableColumn id="17" name="PostFiltersValues" dataDxfId="18"/>
+    <tableColumn id="13" name="PaymentMode" dataDxfId="23"/>
+    <tableColumn id="14" name="Supplier" dataDxfId="22"/>
+    <tableColumn id="15" name="UserType" dataDxfId="21"/>
+    <tableColumn id="16" name="PostFilters" dataDxfId="20"/>
+    <tableColumn id="17" name="PostFiltersValues" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q6" totalsRowShown="0" headerRowDxfId="17" tableBorderDxfId="16">
-  <autoFilter ref="A1:Q6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="18" tableBorderDxfId="17">
+  <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Description" dataDxfId="15"/>
-    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="14"/>
+    <tableColumn id="1" name="Description" dataDxfId="16"/>
+    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="15"/>
     <tableColumn id="3" name="TripType"/>
-    <tableColumn id="4" name="AirPortPairs" dataDxfId="13"/>
-    <tableColumn id="5" name="TravelDates" dataDxfId="12"/>
-    <tableColumn id="6" name="Adults" dataDxfId="11"/>
-    <tableColumn id="7" name="Infants" dataDxfId="10"/>
-    <tableColumn id="8" name="Children" dataDxfId="9"/>
-    <tableColumn id="9" name="IncludeNearByAirPorts" dataDxfId="8"/>
-    <tableColumn id="10" name="CabinType" dataDxfId="7"/>
-    <tableColumn id="11" name="NonStopFlight" dataDxfId="6"/>
-    <tableColumn id="12" name="AirLines" dataDxfId="5"/>
-    <tableColumn id="13" name="PaymentMode" dataDxfId="4"/>
-    <tableColumn id="14" name="Supplier" dataDxfId="3"/>
-    <tableColumn id="15" name="UserType" dataDxfId="2"/>
-    <tableColumn id="16" name="PostFilters" dataDxfId="1"/>
-    <tableColumn id="17" name="PostFiltersValues" dataDxfId="0"/>
+    <tableColumn id="4" name="AirPortPairs" dataDxfId="14"/>
+    <tableColumn id="5" name="TravelDates" dataDxfId="13"/>
+    <tableColumn id="6" name="Adults" dataDxfId="12"/>
+    <tableColumn id="7" name="Infants" dataDxfId="11"/>
+    <tableColumn id="8" name="Children" dataDxfId="10"/>
+    <tableColumn id="9" name="IncludeNearByAirPorts" dataDxfId="9"/>
+    <tableColumn id="10" name="CabinType" dataDxfId="8"/>
+    <tableColumn id="11" name="NonStopFlight" dataDxfId="7"/>
+    <tableColumn id="12" name="AirLines" dataDxfId="6"/>
+    <tableColumn id="13" name="PaymentMode" dataDxfId="5"/>
+    <tableColumn id="14" name="Supplier" dataDxfId="4"/>
+    <tableColumn id="15" name="UserType" dataDxfId="3"/>
+    <tableColumn id="16" name="PostFilters" dataDxfId="2"/>
+    <tableColumn id="17" name="PostFiltersValues" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1843,10 +1705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1882,7 +1744,7 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
@@ -1894,13 +1756,13 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="13" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="13" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="5" t="s">
@@ -1927,16 +1789,16 @@
         <v>17</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="15" t="s">
         <v>20</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>21</v>
       </c>
       <c r="F2" s="8">
         <v>1</v>
@@ -1947,360 +1809,27 @@
       <c r="H2" s="8">
         <v>0</v>
       </c>
-      <c r="I2" s="18" t="b">
+      <c r="I2" s="15" t="b">
         <v>0</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="18" t="b">
+        <v>21</v>
+      </c>
+      <c r="K2" s="15" t="b">
         <v>0</v>
       </c>
       <c r="L2" s="9"/>
       <c r="M2" s="10" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="N2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="20"/>
+      <c r="P2" s="17"/>
       <c r="Q2" s="2"/>
-    </row>
-    <row r="3" spans="1:17" ht="153" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="18">
-        <v>25</v>
-      </c>
-      <c r="F3" s="12">
-        <v>1</v>
-      </c>
-      <c r="G3" s="12">
-        <v>0</v>
-      </c>
-      <c r="H3" s="12">
-        <v>1</v>
-      </c>
-      <c r="I3" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" s="12"/>
-      <c r="M3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="21"/>
-    </row>
-    <row r="4" spans="1:17" ht="153" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="18">
-        <v>25</v>
-      </c>
-      <c r="F4" s="12">
-        <v>1</v>
-      </c>
-      <c r="G4" s="12">
-        <v>1</v>
-      </c>
-      <c r="H4" s="12">
-        <v>0</v>
-      </c>
-      <c r="I4" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="12"/>
-      <c r="M4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="21"/>
-    </row>
-    <row r="5" spans="1:17" ht="102" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="18">
-        <v>25</v>
-      </c>
-      <c r="F5" s="7">
-        <v>1</v>
-      </c>
-      <c r="G5" s="7">
-        <v>1</v>
-      </c>
-      <c r="H5" s="7">
-        <v>1</v>
-      </c>
-      <c r="I5" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q5" s="21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="18">
-        <v>25</v>
-      </c>
-      <c r="F6" s="7">
-        <v>1</v>
-      </c>
-      <c r="G6" s="7">
-        <v>0</v>
-      </c>
-      <c r="H6" s="7">
-        <v>0</v>
-      </c>
-      <c r="I6" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O6" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="21"/>
-    </row>
-    <row r="7" spans="1:17" ht="102" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="18">
-        <v>25</v>
-      </c>
-      <c r="F7" s="7">
-        <v>1</v>
-      </c>
-      <c r="G7" s="7">
-        <v>0</v>
-      </c>
-      <c r="H7" s="7">
-        <v>1</v>
-      </c>
-      <c r="I7" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N7" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O7" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="21"/>
-    </row>
-    <row r="8" spans="1:17" ht="102" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="18">
-        <v>25</v>
-      </c>
-      <c r="F8" s="7">
-        <v>1</v>
-      </c>
-      <c r="G8" s="7">
-        <v>1</v>
-      </c>
-      <c r="H8" s="7">
-        <v>0</v>
-      </c>
-      <c r="I8" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8" s="7"/>
-      <c r="M8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N8" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O8" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="21"/>
-    </row>
-    <row r="9" spans="1:17" ht="102" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="18">
-        <v>25</v>
-      </c>
-      <c r="F9" s="8">
-        <v>1</v>
-      </c>
-      <c r="G9" s="8">
-        <v>1</v>
-      </c>
-      <c r="H9" s="8">
-        <v>1</v>
-      </c>
-      <c r="I9" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L9" s="8"/>
-      <c r="M9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N9" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O9" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2312,10 +1841,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2351,7 +1880,7 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
@@ -2363,13 +1892,13 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="13" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="13" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="5" t="s">
@@ -2393,19 +1922,19 @@
     </row>
     <row r="2" spans="1:17" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>35</v>
+        <v>25</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>28</v>
       </c>
       <c r="F2" s="12">
         <v>1</v>
@@ -2416,223 +1945,31 @@
       <c r="H2" s="12">
         <v>0</v>
       </c>
-      <c r="I2" s="18" t="b">
+      <c r="I2" s="15" t="b">
         <v>0</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="17" t="b">
+        <v>21</v>
+      </c>
+      <c r="K2" s="14" t="b">
         <v>0</v>
       </c>
       <c r="L2" s="12"/>
       <c r="M2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="O2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="11" t="s">
-        <v>25</v>
-      </c>
       <c r="P2" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" s="21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="153" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="12">
-        <v>1</v>
-      </c>
-      <c r="G3" s="12">
-        <v>0</v>
-      </c>
-      <c r="H3" s="12">
-        <v>1</v>
-      </c>
-      <c r="I3" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" s="12"/>
-      <c r="M3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q3" s="21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="153" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="7">
-        <v>1</v>
-      </c>
-      <c r="G4" s="7">
-        <v>1</v>
-      </c>
-      <c r="H4" s="7">
-        <v>0</v>
-      </c>
-      <c r="I4" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="7"/>
-      <c r="M4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="21"/>
-    </row>
-    <row r="5" spans="1:17" ht="165.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="7">
-        <v>1</v>
-      </c>
-      <c r="G5" s="7">
-        <v>1</v>
-      </c>
-      <c r="H5" s="7">
-        <v>1</v>
-      </c>
-      <c r="I5" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="21"/>
-    </row>
-    <row r="6" spans="1:17" s="27" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="8">
-        <v>1</v>
-      </c>
-      <c r="G6" s="8">
-        <v>0</v>
-      </c>
-      <c r="H6" s="8">
-        <v>0</v>
-      </c>
-      <c r="I6" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="L6" s="8"/>
-      <c r="M6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O6" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2644,10 +1981,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2670,74 +2007,74 @@
     <col min="17" max="17" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="O1" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="P1" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="26" t="s">
+      <c r="Q1" s="23" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>48</v>
+        <v>33</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="F2" s="7">
         <v>1</v>
@@ -2748,215 +2085,27 @@
       <c r="H2" s="7">
         <v>0</v>
       </c>
-      <c r="I2" s="18" t="b">
+      <c r="I2" s="15" t="b">
         <v>0</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="17" t="b">
+        <v>21</v>
+      </c>
+      <c r="K2" s="14" t="b">
         <v>0</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="O2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="11" t="s">
-        <v>25</v>
-      </c>
       <c r="P2" s="7"/>
-      <c r="Q2" s="21"/>
-    </row>
-    <row r="3" spans="1:17" ht="140.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="8">
-        <v>1</v>
-      </c>
-      <c r="G3" s="8">
-        <v>0</v>
-      </c>
-      <c r="H3" s="8">
-        <v>1</v>
-      </c>
-      <c r="I3" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="21"/>
-    </row>
-    <row r="4" spans="1:17" ht="153" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="7">
-        <v>1</v>
-      </c>
-      <c r="G4" s="7">
-        <v>1</v>
-      </c>
-      <c r="H4" s="7">
-        <v>0</v>
-      </c>
-      <c r="I4" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="7"/>
-      <c r="M4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="21"/>
-    </row>
-    <row r="5" spans="1:17" ht="165.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="7">
-        <v>1</v>
-      </c>
-      <c r="G5" s="7">
-        <v>1</v>
-      </c>
-      <c r="H5" s="7">
-        <v>1</v>
-      </c>
-      <c r="I5" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="21"/>
-    </row>
-    <row r="6" spans="1:17" s="27" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="8">
-        <v>1</v>
-      </c>
-      <c r="G6" s="8">
-        <v>0</v>
-      </c>
-      <c r="H6" s="8">
-        <v>0</v>
-      </c>
-      <c r="I6" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="L6" s="8"/>
-      <c r="M6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O6" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="9"/>
+      <c r="Q2" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
one test case enabled
testing for jenkins configuration
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/Air/Air_Amadeus.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/Air/Air_Amadeus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="Air_Amadeus_OneWay" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="38">
   <si>
     <t>Description</t>
   </si>
@@ -127,13 +127,16 @@
   </si>
   <si>
     <t>RoviaBucks</t>
+  </si>
+  <si>
+    <t>Guest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +156,16 @@
       <sz val="10"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -175,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -303,11 +316,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -359,30 +383,17 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="50">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -936,6 +947,25 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1341,8 +1371,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="49" headerRowBorderDxfId="48">
-  <autoFilter ref="A1:Q2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q3" totalsRowShown="0" headerRowDxfId="49" headerRowBorderDxfId="48">
+  <autoFilter ref="A1:Q3"/>
   <tableColumns count="17">
     <tableColumn id="1" name="Description" dataDxfId="47"/>
     <tableColumn id="2" name="ExecutionPipeline" dataDxfId="46"/>
@@ -1371,48 +1401,48 @@
   <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
     <tableColumn id="1" name="Description" dataDxfId="30"/>
-    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="0"/>
-    <tableColumn id="3" name="TripType" dataDxfId="29"/>
-    <tableColumn id="4" name="AirPortPairs" dataDxfId="28"/>
-    <tableColumn id="5" name="TravelDates" dataDxfId="27"/>
+    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="29"/>
+    <tableColumn id="3" name="TripType" dataDxfId="28"/>
+    <tableColumn id="4" name="AirPortPairs" dataDxfId="27"/>
+    <tableColumn id="5" name="TravelDates" dataDxfId="26"/>
     <tableColumn id="6" name="Adults"/>
     <tableColumn id="7" name="Infants"/>
     <tableColumn id="8" name="Children"/>
-    <tableColumn id="9" name="IncludeNearByAirPorts" dataDxfId="26"/>
-    <tableColumn id="10" name="CabinType" dataDxfId="25"/>
-    <tableColumn id="11" name="NonStopFlight" dataDxfId="24"/>
+    <tableColumn id="9" name="IncludeNearByAirPorts" dataDxfId="25"/>
+    <tableColumn id="10" name="CabinType" dataDxfId="24"/>
+    <tableColumn id="11" name="NonStopFlight" dataDxfId="23"/>
     <tableColumn id="12" name="AirLines"/>
-    <tableColumn id="13" name="PaymentMode" dataDxfId="23"/>
-    <tableColumn id="14" name="Supplier" dataDxfId="22"/>
-    <tableColumn id="15" name="UserType" dataDxfId="21"/>
-    <tableColumn id="16" name="PostFilters" dataDxfId="20"/>
-    <tableColumn id="17" name="PostFiltersValues" dataDxfId="19"/>
+    <tableColumn id="13" name="PaymentMode" dataDxfId="22"/>
+    <tableColumn id="14" name="Supplier" dataDxfId="21"/>
+    <tableColumn id="15" name="UserType" dataDxfId="20"/>
+    <tableColumn id="16" name="PostFilters" dataDxfId="19"/>
+    <tableColumn id="17" name="PostFiltersValues" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="18" tableBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="17" tableBorderDxfId="16">
   <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Description" dataDxfId="16"/>
-    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="15"/>
+    <tableColumn id="1" name="Description" dataDxfId="15"/>
+    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="14"/>
     <tableColumn id="3" name="TripType"/>
-    <tableColumn id="4" name="AirPortPairs" dataDxfId="14"/>
-    <tableColumn id="5" name="TravelDates" dataDxfId="13"/>
-    <tableColumn id="6" name="Adults" dataDxfId="12"/>
-    <tableColumn id="7" name="Infants" dataDxfId="11"/>
-    <tableColumn id="8" name="Children" dataDxfId="10"/>
-    <tableColumn id="9" name="IncludeNearByAirPorts" dataDxfId="9"/>
-    <tableColumn id="10" name="CabinType" dataDxfId="8"/>
-    <tableColumn id="11" name="NonStopFlight" dataDxfId="7"/>
-    <tableColumn id="12" name="AirLines" dataDxfId="6"/>
-    <tableColumn id="13" name="PaymentMode" dataDxfId="5"/>
-    <tableColumn id="14" name="Supplier" dataDxfId="4"/>
-    <tableColumn id="15" name="UserType" dataDxfId="3"/>
-    <tableColumn id="16" name="PostFilters" dataDxfId="2"/>
-    <tableColumn id="17" name="PostFiltersValues" dataDxfId="1"/>
+    <tableColumn id="4" name="AirPortPairs" dataDxfId="13"/>
+    <tableColumn id="5" name="TravelDates" dataDxfId="12"/>
+    <tableColumn id="6" name="Adults" dataDxfId="11"/>
+    <tableColumn id="7" name="Infants" dataDxfId="10"/>
+    <tableColumn id="8" name="Children" dataDxfId="9"/>
+    <tableColumn id="9" name="IncludeNearByAirPorts" dataDxfId="8"/>
+    <tableColumn id="10" name="CabinType" dataDxfId="7"/>
+    <tableColumn id="11" name="NonStopFlight" dataDxfId="6"/>
+    <tableColumn id="12" name="AirLines" dataDxfId="5"/>
+    <tableColumn id="13" name="PaymentMode" dataDxfId="4"/>
+    <tableColumn id="14" name="Supplier" dataDxfId="3"/>
+    <tableColumn id="15" name="UserType" dataDxfId="2"/>
+    <tableColumn id="16" name="PostFilters" dataDxfId="1"/>
+    <tableColumn id="17" name="PostFiltersValues" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1705,10 +1735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,6 +1860,53 @@
       </c>
       <c r="P2" s="17"/>
       <c r="Q2" s="2"/>
+    </row>
+    <row r="3" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8">
+        <v>0</v>
+      </c>
+      <c r="I3" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" s="8"/>
+      <c r="M3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1983,8 +2060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
code change for analysing failure test report
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/Air/Air_Amadeus.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/Air/Air_Amadeus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Air_Amadeus_OneWay" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="38">
   <si>
     <t>Description</t>
   </si>
@@ -117,12 +117,6 @@
     <t>MultiCity</t>
   </si>
   <si>
-    <t>LAS-LAX|LAX-DFW|DFW-MIA</t>
-  </si>
-  <si>
-    <t>53|64|71</t>
-  </si>
-  <si>
     <t>Search|AddToCart|CHECKOUTTRIP|LOGIN|ENTERPAXINFO|CONFIRMPAXINFO</t>
   </si>
   <si>
@@ -130,6 +124,12 @@
   </si>
   <si>
     <t>Guest</t>
+  </si>
+  <si>
+    <t>LAS-LAX|LAX-DFW|DFW-MIA|MIA-DEL</t>
+  </si>
+  <si>
+    <t>53|64|71|80</t>
   </si>
 </sst>
 </file>
@@ -1423,8 +1423,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="17" tableBorderDxfId="16">
-  <autoFilter ref="A1:Q2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q3" totalsRowShown="0" headerRowDxfId="17" tableBorderDxfId="16">
+  <autoFilter ref="A1:Q3"/>
   <tableColumns count="17">
     <tableColumn id="1" name="Description" dataDxfId="15"/>
     <tableColumn id="2" name="ExecutionPipeline" dataDxfId="14"/>
@@ -1737,7 +1737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -1819,7 +1819,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>18</v>
@@ -1850,7 +1850,7 @@
       </c>
       <c r="L2" s="9"/>
       <c r="M2" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>23</v>
@@ -1866,7 +1866,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>18</v>
@@ -1897,13 +1897,13 @@
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N3" s="10" t="s">
         <v>23</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="P3" s="8"/>
       <c r="Q3" s="9"/>
@@ -2002,7 +2002,7 @@
         <v>26</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>27</v>
@@ -2058,10 +2058,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2142,16 +2142,16 @@
         <v>31</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F2" s="7">
         <v>1</v>
@@ -2183,6 +2183,53 @@
       </c>
       <c r="P2" s="7"/>
       <c r="Q2" s="18"/>
+    </row>
+    <row r="3" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8">
+        <v>1</v>
+      </c>
+      <c r="I3" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" s="8"/>
+      <c r="M3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
enabled all suppliers test cases
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/Air/Air_Amadeus.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/Air/Air_Amadeus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="Air_Amadeus_OneWay" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="37">
   <si>
     <t>Description</t>
   </si>
@@ -121,9 +121,6 @@
   </si>
   <si>
     <t>RoviaBucks</t>
-  </si>
-  <si>
-    <t>Guest</t>
   </si>
   <si>
     <t>LAS-LAX|LAX-DFW|DFW-MIA|MIA-DEL</t>
@@ -136,7 +133,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,16 +153,6 @@
       <sz val="10"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Tahoma"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -188,7 +175,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -316,22 +303,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -383,12 +359,6 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1371,8 +1341,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q3" totalsRowShown="0" headerRowDxfId="49" headerRowBorderDxfId="48">
-  <autoFilter ref="A1:Q3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="49" headerRowBorderDxfId="48">
+  <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
     <tableColumn id="1" name="Description" dataDxfId="47"/>
     <tableColumn id="2" name="ExecutionPipeline" dataDxfId="46"/>
@@ -1423,8 +1393,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q3" totalsRowShown="0" headerRowDxfId="17" tableBorderDxfId="16">
-  <autoFilter ref="A1:Q3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="17" tableBorderDxfId="16">
+  <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
     <tableColumn id="1" name="Description" dataDxfId="15"/>
     <tableColumn id="2" name="ExecutionPipeline" dataDxfId="14"/>
@@ -1735,10 +1705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1860,53 +1830,6 @@
       </c>
       <c r="P2" s="17"/>
       <c r="Q2" s="2"/>
-    </row>
-    <row r="3" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="8">
-        <v>1</v>
-      </c>
-      <c r="G3" s="8">
-        <v>0</v>
-      </c>
-      <c r="H3" s="8">
-        <v>0</v>
-      </c>
-      <c r="I3" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2058,10 +1981,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2148,10 +2071,10 @@
         <v>32</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>36</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>37</v>
       </c>
       <c r="F2" s="7">
         <v>1</v>
@@ -2183,53 +2106,6 @@
       </c>
       <c r="P2" s="7"/>
       <c r="Q2" s="18"/>
-    </row>
-    <row r="3" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="8">
-        <v>1</v>
-      </c>
-      <c r="G3" s="8">
-        <v>0</v>
-      </c>
-      <c r="H3" s="8">
-        <v>1</v>
-      </c>
-      <c r="I3" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
tripfolder pages for car folder
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/Air/Air_Amadeus.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/Air/Air_Amadeus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Air_Amadeus_OneWay" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="58">
   <si>
     <t>Description</t>
   </si>
@@ -120,9 +120,6 @@
     <t>RoviaBucks</t>
   </si>
   <si>
-    <t>AmadeusWS air oneway booking for DOMESTIC location for 1 Adult with Guest Login</t>
-  </si>
-  <si>
     <t>Guest</t>
   </si>
   <si>
@@ -133,13 +130,73 @@
   </si>
   <si>
     <t>Search|AddToCart|CHECKOUTTRIP|LOGIN|ENTERPAXINFO|CONFIRMPAXINFO</t>
+  </si>
+  <si>
+    <t>AmadeusWS air oneway booking for DOMESTIC location for 1 Adult and 1 child with Login.</t>
+  </si>
+  <si>
+    <t>AmadeusWS air oneway booking for DOMESTIC location for 1 adult and 1 infant with Login.</t>
+  </si>
+  <si>
+    <t>AmadeusWS air oneway booking for DOMESTIC location for 1 adult . 1 child and 1 infant with Login.</t>
+  </si>
+  <si>
+    <t>airlines</t>
+  </si>
+  <si>
+    <t>AA/NK</t>
+  </si>
+  <si>
+    <t>AmadeusWS air oneway booking for INTERNATIONAL location for 1 Adult with Login.</t>
+  </si>
+  <si>
+    <t>JFK-PAR</t>
+  </si>
+  <si>
+    <t>AmadeusWS air oneway booking for INTERNATIONAL location 1 Adult and 1 child with Login.</t>
+  </si>
+  <si>
+    <t>AmadeusWS air oneway booking for INTERNATIONAL location for 1 adult and 1 infant with Login.</t>
+  </si>
+  <si>
+    <t>AmadeusWS air oneway booking for INTERNATIONAL location for 1 adult. 1 child and 1 infant with Login.</t>
+  </si>
+  <si>
+    <t>AmadeusWS air round trip booking for DOMESTIC location for 1 adult and 1 child with Login.</t>
+  </si>
+  <si>
+    <t>stop|cabin</t>
+  </si>
+  <si>
+    <t>one|business</t>
+  </si>
+  <si>
+    <t>AmadeusWS air round trip booking for DOMESTIC location for 1 adult and 1 infant with Login.</t>
+  </si>
+  <si>
+    <t>Search|AddToCart|CHECKOUTTRIP|LOGIN|ENTERPAXINFO|CONFIRMPAXINFO|PAYNOW</t>
+  </si>
+  <si>
+    <t>AmadeusWS air round trip booking for DOMESTIC location for 1 adult. 1 child and 1 infant with Login.</t>
+  </si>
+  <si>
+    <t>DFW-LAS</t>
+  </si>
+  <si>
+    <t>AmadeusWS air MULTICITY booking for DOMESTIC location 1 Adult and 1 child with Login.</t>
+  </si>
+  <si>
+    <t>AmadeusWS air MULTICITY booking for DOMESTIC location for 1 adult and 1 infant with Login.</t>
+  </si>
+  <si>
+    <t>AmadeusWS air MULTICITY booking for DOMESTIC location for 1 adult .1 child and 1 infant with Login.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,16 +216,6 @@
       <sz val="10"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Tahoma"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -191,7 +238,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -330,11 +377,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -386,34 +461,23 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="50">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -967,6 +1031,23 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1372,8 +1453,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q3" totalsRowShown="0" headerRowDxfId="49" headerRowBorderDxfId="48">
-  <autoFilter ref="A1:Q3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="49" headerRowBorderDxfId="48">
+  <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
     <tableColumn id="1" name="Description" dataDxfId="47"/>
     <tableColumn id="2" name="ExecutionPipeline" dataDxfId="46"/>
@@ -1402,48 +1483,48 @@
   <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
     <tableColumn id="1" name="Description" dataDxfId="30"/>
-    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="0"/>
-    <tableColumn id="3" name="TripType" dataDxfId="29"/>
-    <tableColumn id="4" name="AirPortPairs" dataDxfId="28"/>
-    <tableColumn id="5" name="TravelDates" dataDxfId="27"/>
+    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="29"/>
+    <tableColumn id="3" name="TripType" dataDxfId="28"/>
+    <tableColumn id="4" name="AirPortPairs" dataDxfId="27"/>
+    <tableColumn id="5" name="TravelDates" dataDxfId="26"/>
     <tableColumn id="6" name="Adults"/>
     <tableColumn id="7" name="Infants"/>
     <tableColumn id="8" name="Children"/>
-    <tableColumn id="9" name="IncludeNearByAirPorts" dataDxfId="26"/>
-    <tableColumn id="10" name="CabinType" dataDxfId="25"/>
-    <tableColumn id="11" name="NonStopFlight" dataDxfId="24"/>
+    <tableColumn id="9" name="IncludeNearByAirPorts" dataDxfId="25"/>
+    <tableColumn id="10" name="CabinType" dataDxfId="24"/>
+    <tableColumn id="11" name="NonStopFlight" dataDxfId="23"/>
     <tableColumn id="12" name="AirLines"/>
-    <tableColumn id="13" name="PaymentMode" dataDxfId="23"/>
-    <tableColumn id="14" name="Supplier" dataDxfId="22"/>
-    <tableColumn id="15" name="UserType" dataDxfId="21"/>
-    <tableColumn id="16" name="PostFilters" dataDxfId="20"/>
-    <tableColumn id="17" name="PostFiltersValues" dataDxfId="19"/>
+    <tableColumn id="13" name="PaymentMode" dataDxfId="22"/>
+    <tableColumn id="14" name="Supplier" dataDxfId="21"/>
+    <tableColumn id="15" name="UserType" dataDxfId="20"/>
+    <tableColumn id="16" name="PostFilters" dataDxfId="19"/>
+    <tableColumn id="17" name="PostFiltersValues" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q3" totalsRowShown="0" headerRowDxfId="18" tableBorderDxfId="17">
-  <autoFilter ref="A1:Q3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="17" tableBorderDxfId="16">
+  <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Description" dataDxfId="16"/>
-    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="15"/>
+    <tableColumn id="1" name="Description" dataDxfId="15"/>
+    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="14"/>
     <tableColumn id="3" name="TripType"/>
-    <tableColumn id="4" name="AirPortPairs" dataDxfId="14"/>
-    <tableColumn id="5" name="TravelDates" dataDxfId="13"/>
-    <tableColumn id="6" name="Adults" dataDxfId="12"/>
-    <tableColumn id="7" name="Infants" dataDxfId="11"/>
-    <tableColumn id="8" name="Children" dataDxfId="10"/>
-    <tableColumn id="9" name="IncludeNearByAirPorts" dataDxfId="9"/>
-    <tableColumn id="10" name="CabinType" dataDxfId="8"/>
-    <tableColumn id="11" name="NonStopFlight" dataDxfId="7"/>
-    <tableColumn id="12" name="AirLines" dataDxfId="6"/>
-    <tableColumn id="13" name="PaymentMode" dataDxfId="5"/>
-    <tableColumn id="14" name="Supplier" dataDxfId="4"/>
-    <tableColumn id="15" name="UserType" dataDxfId="3"/>
-    <tableColumn id="16" name="PostFilters" dataDxfId="2"/>
-    <tableColumn id="17" name="PostFiltersValues" dataDxfId="1"/>
+    <tableColumn id="4" name="AirPortPairs" dataDxfId="13"/>
+    <tableColumn id="5" name="TravelDates" dataDxfId="12"/>
+    <tableColumn id="6" name="Adults" dataDxfId="11"/>
+    <tableColumn id="7" name="Infants" dataDxfId="10"/>
+    <tableColumn id="8" name="Children" dataDxfId="9"/>
+    <tableColumn id="9" name="IncludeNearByAirPorts" dataDxfId="8"/>
+    <tableColumn id="10" name="CabinType" dataDxfId="7"/>
+    <tableColumn id="11" name="NonStopFlight" dataDxfId="6"/>
+    <tableColumn id="12" name="AirLines" dataDxfId="5"/>
+    <tableColumn id="13" name="PaymentMode" dataDxfId="4"/>
+    <tableColumn id="14" name="Supplier" dataDxfId="3"/>
+    <tableColumn id="15" name="UserType" dataDxfId="2"/>
+    <tableColumn id="16" name="PostFilters" dataDxfId="1"/>
+    <tableColumn id="17" name="PostFiltersValues" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1736,10 +1817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1820,7 +1901,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>18</v>
@@ -1862,52 +1943,338 @@
       <c r="P2" s="17"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="1:17" s="1" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="B3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="8">
-        <v>1</v>
-      </c>
-      <c r="G3" s="8">
-        <v>0</v>
-      </c>
-      <c r="H3" s="8">
-        <v>0</v>
-      </c>
-      <c r="I3" s="15" t="b">
+        <v>25</v>
+      </c>
+      <c r="E3" s="15">
+        <v>25</v>
+      </c>
+      <c r="F3" s="12">
+        <v>1</v>
+      </c>
+      <c r="G3" s="12">
+        <v>0</v>
+      </c>
+      <c r="H3" s="12">
+        <v>1</v>
+      </c>
+      <c r="I3" s="16" t="b">
         <v>0</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" s="8"/>
+      <c r="K3" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" s="12"/>
       <c r="M3" s="10" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="N3" s="10" t="s">
         <v>23</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="18"/>
+    </row>
+    <row r="4" spans="1:17" s="1" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="15">
+        <v>25</v>
+      </c>
+      <c r="F4" s="12">
+        <v>1</v>
+      </c>
+      <c r="G4" s="12">
+        <v>1</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0</v>
+      </c>
+      <c r="I4" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" s="12"/>
+      <c r="M4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="18"/>
+    </row>
+    <row r="5" spans="1:17" s="1" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="15">
+        <v>25</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
+      <c r="G5" s="7">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7">
+        <v>1</v>
+      </c>
+      <c r="I5" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="7"/>
+      <c r="M5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q5" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" s="1" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="15">
+        <v>25</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0</v>
+      </c>
+      <c r="I6" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" s="7"/>
+      <c r="M6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="18"/>
+    </row>
+    <row r="7" spans="1:17" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="15">
+        <v>25</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" s="7"/>
+      <c r="M7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="18"/>
+    </row>
+    <row r="8" spans="1:17" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="15">
+        <v>25</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1</v>
+      </c>
+      <c r="G8" s="7">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0</v>
+      </c>
+      <c r="I8" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" s="7"/>
+      <c r="M8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="18"/>
+    </row>
+    <row r="9" spans="1:17" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="15">
+        <v>25</v>
+      </c>
+      <c r="F9" s="8">
+        <v>1</v>
+      </c>
+      <c r="G9" s="8">
+        <v>1</v>
+      </c>
+      <c r="H9" s="8">
+        <v>1</v>
+      </c>
+      <c r="I9" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" s="8"/>
+      <c r="M9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1919,10 +2286,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2003,7 +2370,7 @@
         <v>26</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>27</v>
@@ -2048,6 +2415,151 @@
       <c r="Q2" s="18" t="s">
         <v>30</v>
       </c>
+    </row>
+    <row r="3" spans="1:17" s="1" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="12">
+        <v>1</v>
+      </c>
+      <c r="G3" s="12">
+        <v>0</v>
+      </c>
+      <c r="H3" s="12">
+        <v>1</v>
+      </c>
+      <c r="I3" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" s="12"/>
+      <c r="M3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q3" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1</v>
+      </c>
+      <c r="G4" s="7">
+        <v>1</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" s="7"/>
+      <c r="M4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="18"/>
+    </row>
+    <row r="5" spans="1:17" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
+      <c r="G5" s="7">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7">
+        <v>1</v>
+      </c>
+      <c r="I5" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="7"/>
+      <c r="M5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2059,10 +2571,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2143,16 +2655,16 @@
         <v>31</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>36</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>37</v>
       </c>
       <c r="F2" s="7">
         <v>1</v>
@@ -2185,22 +2697,22 @@
       <c r="P2" s="7"/>
       <c r="Q2" s="18"/>
     </row>
-    <row r="3" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="8" t="s">
+    <row r="3" spans="1:17" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="15" t="s">
-        <v>37</v>
-      </c>
       <c r="F3" s="8">
         <v>1</v>
       </c>
@@ -2208,7 +2720,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="15" t="b">
         <v>0</v>
@@ -2216,12 +2728,12 @@
       <c r="J3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="15" t="b">
+      <c r="K3" s="14" t="b">
         <v>0</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="10" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="N3" s="10" t="s">
         <v>23</v>
@@ -2229,8 +2741,102 @@
       <c r="O3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="9"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="18"/>
+    </row>
+    <row r="4" spans="1:17" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1</v>
+      </c>
+      <c r="G4" s="7">
+        <v>1</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" s="7"/>
+      <c r="M4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="18"/>
+    </row>
+    <row r="5" spans="1:17" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
+      <c r="G5" s="7">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7">
+        <v>1</v>
+      </c>
+      <c r="I5" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="7"/>
+      <c r="M5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix for AddToCart method and added BookNow function for car product
Also changes for datasheet files
added multiple scenarios for air supplier lists
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/Air/Air_Amadeus.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/Air/Air_Amadeus.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="61">
   <si>
     <t>Description</t>
   </si>
@@ -174,9 +174,6 @@
     <t>AmadeusWS air round trip booking for DOMESTIC location for 1 adult and 1 infant with Login.</t>
   </si>
   <si>
-    <t>Search|AddToCart|CHECKOUTTRIP|LOGIN|ENTERPAXINFO|CONFIRMPAXINFO|PAYNOW</t>
-  </si>
-  <si>
     <t>AmadeusWS air round trip booking for DOMESTIC location for 1 adult. 1 child and 1 infant with Login.</t>
   </si>
   <si>
@@ -190,6 +187,18 @@
   </si>
   <si>
     <t>AmadeusWS air MULTICITY booking for DOMESTIC location for 1 adult .1 child and 1 infant with Login.</t>
+  </si>
+  <si>
+    <t>AmadeusWS air round trip booking for INTERNATIONAL location for 1 Adult with Login.</t>
+  </si>
+  <si>
+    <t>AmadeusWS air MULTICITY booking for INTERNATIONAL location for 1 Adult with Login.</t>
+  </si>
+  <si>
+    <t>SIN-BKK|BKK-SIN|SIN-HKG</t>
+  </si>
+  <si>
+    <t>12|20|22</t>
   </si>
 </sst>
 </file>
@@ -1819,8 +1828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2286,10 +2295,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2472,7 +2481,7 @@
         <v>51</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>27</v>
@@ -2516,7 +2525,7 @@
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="26" t="s">
         <v>37</v>
@@ -2525,7 +2534,7 @@
         <v>27</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>28</v>
@@ -2560,6 +2569,53 @@
       </c>
       <c r="P5" s="7"/>
       <c r="Q5" s="18"/>
+    </row>
+    <row r="6" spans="1:17" s="1" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0</v>
+      </c>
+      <c r="I6" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" s="7"/>
+      <c r="M6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2571,10 +2627,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2699,7 +2755,7 @@
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="26" t="s">
         <v>37</v>
@@ -2746,7 +2802,7 @@
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>37</v>
@@ -2793,7 +2849,7 @@
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>37</v>
@@ -2837,6 +2893,53 @@
       </c>
       <c r="P5" s="7"/>
       <c r="Q5" s="18"/>
+    </row>
+    <row r="6" spans="1:17" s="1" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0</v>
+      </c>
+      <c r="I6" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" s="7"/>
+      <c r="M6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Car and Air datasheets
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/Air/Air_Amadeus.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/Air/Air_Amadeus.xlsx
@@ -2629,8 +2629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2647,7 +2647,7 @@
     <col min="11" max="11" width="15.85546875" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" customWidth="1"/>
     <col min="13" max="13" width="16.28515625" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.5703125" customWidth="1"/>
     <col min="16" max="16" width="12.5703125" customWidth="1"/>
     <col min="17" max="17" width="18.5703125" customWidth="1"/>
@@ -2737,9 +2737,7 @@
       <c r="J2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="14" t="b">
-        <v>0</v>
-      </c>
+      <c r="K2" s="14"/>
       <c r="L2" s="7"/>
       <c r="M2" s="10" t="s">
         <v>22</v>
@@ -2784,9 +2782,7 @@
       <c r="J3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="14" t="b">
-        <v>0</v>
-      </c>
+      <c r="K3" s="14"/>
       <c r="L3" s="8"/>
       <c r="M3" s="10" t="s">
         <v>33</v>
@@ -2831,9 +2827,7 @@
       <c r="J4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="14" t="b">
-        <v>0</v>
-      </c>
+      <c r="K4" s="14"/>
       <c r="L4" s="7"/>
       <c r="M4" s="10" t="s">
         <v>22</v>
@@ -2878,9 +2872,7 @@
       <c r="J5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="14" t="b">
-        <v>0</v>
-      </c>
+      <c r="K5" s="14"/>
       <c r="L5" s="7"/>
       <c r="M5" s="10" t="s">
         <v>22</v>
@@ -2925,9 +2917,7 @@
       <c r="J6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="14" t="b">
-        <v>0</v>
-      </c>
+      <c r="K6" s="14"/>
       <c r="L6" s="7"/>
       <c r="M6" s="10" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
added validations for added itinerary for air product
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/Air/Air_Amadeus.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/Air/Air_Amadeus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Air_Amadeus_OneWay" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="68">
   <si>
     <t>Description</t>
   </si>
@@ -105,12 +105,6 @@
     <t>25|32</t>
   </si>
   <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>20-30</t>
-  </si>
-  <si>
     <t>AmadeusWS air MULTICITY booking for DOMESTIC location for 1 Adult with Login.</t>
   </si>
   <si>
@@ -141,12 +135,6 @@
     <t>AmadeusWS air oneway booking for DOMESTIC location for 1 adult . 1 child and 1 infant with Login.</t>
   </si>
   <si>
-    <t>airlines</t>
-  </si>
-  <si>
-    <t>AA/NK</t>
-  </si>
-  <si>
     <t>AmadeusWS air oneway booking for INTERNATIONAL location for 1 Adult with Login.</t>
   </si>
   <si>
@@ -168,9 +156,6 @@
     <t>stop|cabin</t>
   </si>
   <si>
-    <t>one|business</t>
-  </si>
-  <si>
     <t>AmadeusWS air round trip booking for DOMESTIC location for 1 adult and 1 infant with Login.</t>
   </si>
   <si>
@@ -199,6 +184,42 @@
   </si>
   <si>
     <t>12|20|22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Airlines </t>
+  </si>
+  <si>
+    <t>Cabin</t>
+  </si>
+  <si>
+    <t>business/Economy</t>
+  </si>
+  <si>
+    <t>price|duration</t>
+  </si>
+  <si>
+    <t>Matrix</t>
+  </si>
+  <si>
+    <t>20-30|18</t>
+  </si>
+  <si>
+    <t>american airlines/us airways/united airlines</t>
+  </si>
+  <si>
+    <t>Search|setfilters|AddToCart</t>
+  </si>
+  <si>
+    <t>Business/Economy</t>
+  </si>
+  <si>
+    <t>Search|setfilters|addtocart</t>
+  </si>
+  <si>
+    <t>matrix</t>
+  </si>
+  <si>
+    <t>one|business/Economy</t>
   </si>
 </sst>
 </file>
@@ -418,12 +439,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -458,9 +476,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -532,6 +547,59 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top/>
         <bottom/>
         <vertical/>
@@ -1102,42 +1170,6 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -1357,25 +1389,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1466,22 +1479,22 @@
   <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
     <tableColumn id="1" name="Description" dataDxfId="47"/>
-    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="46"/>
-    <tableColumn id="3" name="TripType" dataDxfId="45"/>
-    <tableColumn id="4" name="AirPortPairs" dataDxfId="44"/>
-    <tableColumn id="5" name="TravelDates" dataDxfId="43"/>
-    <tableColumn id="6" name="Adults" dataDxfId="42"/>
-    <tableColumn id="7" name="Infants" dataDxfId="41"/>
-    <tableColumn id="8" name="Children" dataDxfId="40"/>
-    <tableColumn id="9" name="IncludeNearByAirPorts" dataDxfId="39"/>
-    <tableColumn id="10" name="CabinType" dataDxfId="38"/>
-    <tableColumn id="11" name="NonStopFlight" dataDxfId="37"/>
-    <tableColumn id="12" name="AirLines" dataDxfId="36"/>
-    <tableColumn id="13" name="PaymentMode" dataDxfId="35"/>
-    <tableColumn id="14" name="Supplier" dataDxfId="34"/>
-    <tableColumn id="15" name="UserType" dataDxfId="33"/>
-    <tableColumn id="16" name="PostFilters" dataDxfId="32"/>
-    <tableColumn id="17" name="PostFiltersValues" dataDxfId="31"/>
+    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="2"/>
+    <tableColumn id="3" name="TripType" dataDxfId="46"/>
+    <tableColumn id="4" name="AirPortPairs" dataDxfId="45"/>
+    <tableColumn id="5" name="TravelDates" dataDxfId="44"/>
+    <tableColumn id="6" name="Adults" dataDxfId="43"/>
+    <tableColumn id="7" name="Infants" dataDxfId="42"/>
+    <tableColumn id="8" name="Children" dataDxfId="41"/>
+    <tableColumn id="9" name="IncludeNearByAirPorts" dataDxfId="40"/>
+    <tableColumn id="10" name="CabinType" dataDxfId="39"/>
+    <tableColumn id="11" name="NonStopFlight" dataDxfId="38"/>
+    <tableColumn id="12" name="AirLines" dataDxfId="37"/>
+    <tableColumn id="13" name="PaymentMode" dataDxfId="36"/>
+    <tableColumn id="14" name="Supplier" dataDxfId="35"/>
+    <tableColumn id="15" name="UserType" dataDxfId="34"/>
+    <tableColumn id="16" name="PostFilters" dataDxfId="1"/>
+    <tableColumn id="17" name="PostFiltersValues" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1491,49 +1504,49 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:Q2" totalsRowShown="0">
   <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Description" dataDxfId="30"/>
-    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="29"/>
-    <tableColumn id="3" name="TripType" dataDxfId="28"/>
-    <tableColumn id="4" name="AirPortPairs" dataDxfId="27"/>
-    <tableColumn id="5" name="TravelDates" dataDxfId="26"/>
+    <tableColumn id="1" name="Description" dataDxfId="33"/>
+    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="32"/>
+    <tableColumn id="3" name="TripType" dataDxfId="31"/>
+    <tableColumn id="4" name="AirPortPairs" dataDxfId="30"/>
+    <tableColumn id="5" name="TravelDates" dataDxfId="29"/>
     <tableColumn id="6" name="Adults"/>
     <tableColumn id="7" name="Infants"/>
     <tableColumn id="8" name="Children"/>
-    <tableColumn id="9" name="IncludeNearByAirPorts" dataDxfId="25"/>
-    <tableColumn id="10" name="CabinType" dataDxfId="24"/>
-    <tableColumn id="11" name="NonStopFlight" dataDxfId="23"/>
+    <tableColumn id="9" name="IncludeNearByAirPorts" dataDxfId="28"/>
+    <tableColumn id="10" name="CabinType" dataDxfId="27"/>
+    <tableColumn id="11" name="NonStopFlight" dataDxfId="26"/>
     <tableColumn id="12" name="AirLines"/>
-    <tableColumn id="13" name="PaymentMode" dataDxfId="22"/>
-    <tableColumn id="14" name="Supplier" dataDxfId="21"/>
-    <tableColumn id="15" name="UserType" dataDxfId="20"/>
-    <tableColumn id="16" name="PostFilters" dataDxfId="19"/>
-    <tableColumn id="17" name="PostFiltersValues" dataDxfId="18"/>
+    <tableColumn id="13" name="PaymentMode" dataDxfId="25"/>
+    <tableColumn id="14" name="Supplier" dataDxfId="24"/>
+    <tableColumn id="15" name="UserType" dataDxfId="23"/>
+    <tableColumn id="16" name="PostFilters" dataDxfId="22"/>
+    <tableColumn id="17" name="PostFiltersValues" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="17" tableBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="20" tableBorderDxfId="19">
   <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Description" dataDxfId="15"/>
-    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="14"/>
+    <tableColumn id="1" name="Description" dataDxfId="18"/>
+    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="17"/>
     <tableColumn id="3" name="TripType"/>
-    <tableColumn id="4" name="AirPortPairs" dataDxfId="13"/>
-    <tableColumn id="5" name="TravelDates" dataDxfId="12"/>
-    <tableColumn id="6" name="Adults" dataDxfId="11"/>
-    <tableColumn id="7" name="Infants" dataDxfId="10"/>
-    <tableColumn id="8" name="Children" dataDxfId="9"/>
-    <tableColumn id="9" name="IncludeNearByAirPorts" dataDxfId="8"/>
-    <tableColumn id="10" name="CabinType" dataDxfId="7"/>
-    <tableColumn id="11" name="NonStopFlight" dataDxfId="6"/>
-    <tableColumn id="12" name="AirLines" dataDxfId="5"/>
-    <tableColumn id="13" name="PaymentMode" dataDxfId="4"/>
-    <tableColumn id="14" name="Supplier" dataDxfId="3"/>
-    <tableColumn id="15" name="UserType" dataDxfId="2"/>
-    <tableColumn id="16" name="PostFilters" dataDxfId="1"/>
-    <tableColumn id="17" name="PostFiltersValues" dataDxfId="0"/>
+    <tableColumn id="4" name="AirPortPairs" dataDxfId="16"/>
+    <tableColumn id="5" name="TravelDates" dataDxfId="15"/>
+    <tableColumn id="6" name="Adults" dataDxfId="14"/>
+    <tableColumn id="7" name="Infants" dataDxfId="13"/>
+    <tableColumn id="8" name="Children" dataDxfId="12"/>
+    <tableColumn id="9" name="IncludeNearByAirPorts" dataDxfId="11"/>
+    <tableColumn id="10" name="CabinType" dataDxfId="10"/>
+    <tableColumn id="11" name="NonStopFlight" dataDxfId="9"/>
+    <tableColumn id="12" name="AirLines" dataDxfId="8"/>
+    <tableColumn id="13" name="PaymentMode" dataDxfId="7"/>
+    <tableColumn id="14" name="Supplier" dataDxfId="6"/>
+    <tableColumn id="15" name="UserType" dataDxfId="5"/>
+    <tableColumn id="16" name="PostFilters" dataDxfId="4"/>
+    <tableColumn id="17" name="PostFiltersValues" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1828,8 +1841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1853,437 +1866,423 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="8">
-        <v>1</v>
-      </c>
-      <c r="G2" s="8">
-        <v>0</v>
-      </c>
-      <c r="H2" s="8">
-        <v>0</v>
-      </c>
-      <c r="I2" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" s="9"/>
-      <c r="M2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="10" t="s">
+      <c r="F2" s="7">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7">
+        <v>0</v>
+      </c>
+      <c r="I2" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" s="8"/>
+      <c r="M2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="O2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="2"/>
+      <c r="P2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="A3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="14">
         <v>25</v>
       </c>
-      <c r="F3" s="12">
-        <v>1</v>
-      </c>
-      <c r="G3" s="12">
-        <v>0</v>
-      </c>
-      <c r="H3" s="12">
-        <v>1</v>
-      </c>
-      <c r="I3" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" s="12"/>
-      <c r="M3" s="10" t="s">
+      <c r="F3" s="11">
+        <v>1</v>
+      </c>
+      <c r="G3" s="11">
+        <v>0</v>
+      </c>
+      <c r="H3" s="11">
+        <v>1</v>
+      </c>
+      <c r="I3" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" s="11"/>
+      <c r="M3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="18"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="16"/>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="14">
         <v>25</v>
       </c>
-      <c r="F4" s="12">
-        <v>1</v>
-      </c>
-      <c r="G4" s="12">
-        <v>1</v>
-      </c>
-      <c r="H4" s="12">
-        <v>0</v>
-      </c>
-      <c r="I4" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="12"/>
-      <c r="M4" s="10" t="s">
+      <c r="F4" s="11">
+        <v>1</v>
+      </c>
+      <c r="G4" s="11">
+        <v>1</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0</v>
+      </c>
+      <c r="I4" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" s="11"/>
+      <c r="M4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="N4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="O4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="18"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="16"/>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="A5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>25</v>
       </c>
-      <c r="F5" s="7">
-        <v>1</v>
-      </c>
-      <c r="G5" s="7">
-        <v>1</v>
-      </c>
-      <c r="H5" s="7">
-        <v>1</v>
-      </c>
-      <c r="I5" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="10" t="s">
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1</v>
+      </c>
+      <c r="H5" s="6">
+        <v>1</v>
+      </c>
+      <c r="I5" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="7"/>
+      <c r="K5" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6"/>
+      <c r="M5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="N5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="O5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q5" s="18" t="s">
-        <v>42</v>
-      </c>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="16"/>
     </row>
     <row r="6" spans="1:17" s="1" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="12" t="s">
+      <c r="A6" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="15">
+      <c r="D6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="14">
         <v>25</v>
       </c>
-      <c r="F6" s="7">
-        <v>1</v>
-      </c>
-      <c r="G6" s="7">
-        <v>0</v>
-      </c>
-      <c r="H6" s="7">
-        <v>0</v>
-      </c>
-      <c r="I6" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="10" t="s">
+      <c r="F6" s="6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="7"/>
+      <c r="K6" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" s="6"/>
+      <c r="M6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="N6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="O6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="18"/>
+      <c r="P6" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q6" s="16"/>
     </row>
     <row r="7" spans="1:17" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="12" t="s">
+      <c r="A7" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="15">
+      <c r="D7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="14">
         <v>25</v>
       </c>
-      <c r="F7" s="7">
-        <v>1</v>
-      </c>
-      <c r="G7" s="7">
-        <v>0</v>
-      </c>
-      <c r="H7" s="7">
-        <v>1</v>
-      </c>
-      <c r="I7" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="10" t="s">
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6">
+        <v>1</v>
+      </c>
+      <c r="I7" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="7"/>
+      <c r="K7" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" s="6"/>
+      <c r="M7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N7" s="10" t="s">
+      <c r="N7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="11" t="s">
+      <c r="O7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="18"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="16"/>
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="12" t="s">
+      <c r="A8" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="15">
+      <c r="D8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="14">
         <v>25</v>
       </c>
-      <c r="F8" s="7">
-        <v>1</v>
-      </c>
-      <c r="G8" s="7">
-        <v>1</v>
-      </c>
-      <c r="H8" s="7">
-        <v>0</v>
-      </c>
-      <c r="I8" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8" s="7"/>
-      <c r="M8" s="10" t="s">
+      <c r="F8" s="6">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0</v>
+      </c>
+      <c r="I8" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" s="6"/>
+      <c r="M8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N8" s="10" t="s">
+      <c r="N8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O8" s="11" t="s">
+      <c r="O8" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="18"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="16"/>
     </row>
     <row r="9" spans="1:17" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="25" t="s">
+      <c r="A9" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="15">
+      <c r="D9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="14">
         <v>25</v>
       </c>
-      <c r="F9" s="8">
-        <v>1</v>
-      </c>
-      <c r="G9" s="8">
-        <v>1</v>
-      </c>
-      <c r="H9" s="8">
-        <v>1</v>
-      </c>
-      <c r="I9" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="L9" s="8"/>
-      <c r="M9" s="10" t="s">
+      <c r="F9" s="7">
+        <v>1</v>
+      </c>
+      <c r="G9" s="7">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7">
+        <v>1</v>
+      </c>
+      <c r="I9" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" s="7"/>
+      <c r="M9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N9" s="10" t="s">
+      <c r="N9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O9" s="11" t="s">
+      <c r="O9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="18"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2297,8 +2296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2317,305 +2316,305 @@
     <col min="13" max="13" width="16.140625" customWidth="1"/>
     <col min="14" max="14" width="10.5703125" customWidth="1"/>
     <col min="15" max="15" width="11.42578125" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="12">
-        <v>1</v>
-      </c>
-      <c r="G2" s="12">
-        <v>0</v>
-      </c>
-      <c r="H2" s="12">
-        <v>0</v>
-      </c>
-      <c r="I2" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" s="12"/>
-      <c r="M2" s="10" t="s">
+      <c r="F2" s="11">
+        <v>1</v>
+      </c>
+      <c r="G2" s="11">
+        <v>0</v>
+      </c>
+      <c r="H2" s="11">
+        <v>0</v>
+      </c>
+      <c r="I2" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" s="11"/>
+      <c r="M2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="O2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="18" t="s">
-        <v>30</v>
+      <c r="P2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="12" t="s">
+      <c r="A3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="12">
-        <v>1</v>
-      </c>
-      <c r="G3" s="12">
-        <v>0</v>
-      </c>
-      <c r="H3" s="12">
-        <v>1</v>
-      </c>
-      <c r="I3" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" s="12"/>
-      <c r="M3" s="10" t="s">
+      <c r="F3" s="11">
+        <v>1</v>
+      </c>
+      <c r="G3" s="11">
+        <v>0</v>
+      </c>
+      <c r="H3" s="11">
+        <v>1</v>
+      </c>
+      <c r="I3" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" s="11"/>
+      <c r="M3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q3" s="18" t="s">
-        <v>50</v>
+      <c r="P3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q3" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="A4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="7">
-        <v>1</v>
-      </c>
-      <c r="G4" s="7">
-        <v>1</v>
-      </c>
-      <c r="H4" s="7">
-        <v>0</v>
-      </c>
-      <c r="I4" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="7"/>
-      <c r="M4" s="10" t="s">
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6"/>
+      <c r="M4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="N4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="18"/>
+      <c r="O4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="12" t="s">
+      <c r="A5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="16" t="s">
+      <c r="D5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="7">
-        <v>1</v>
-      </c>
-      <c r="G5" s="7">
-        <v>1</v>
-      </c>
-      <c r="H5" s="7">
-        <v>1</v>
-      </c>
-      <c r="I5" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="10" t="s">
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1</v>
+      </c>
+      <c r="H5" s="6">
+        <v>1</v>
+      </c>
+      <c r="I5" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="7"/>
+      <c r="K5" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6"/>
+      <c r="M5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="N5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="O5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="18"/>
+      <c r="P5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q5" s="16" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="6" spans="1:17" s="1" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="12" t="s">
+      <c r="A6" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="16" t="s">
+      <c r="D6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="7">
-        <v>1</v>
-      </c>
-      <c r="G6" s="7">
-        <v>0</v>
-      </c>
-      <c r="H6" s="7">
-        <v>0</v>
-      </c>
-      <c r="I6" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="10" t="s">
+      <c r="F6" s="6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="7"/>
+      <c r="K6" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" s="6"/>
+      <c r="M6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="N6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="O6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
+      <c r="P6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q6" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2629,7 +2628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -2653,279 +2652,279 @@
     <col min="17" max="17" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="21" t="s">
+    <row r="1" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="P1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="Q1" s="21" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="A2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="7">
-        <v>1</v>
-      </c>
-      <c r="G2" s="7">
-        <v>0</v>
-      </c>
-      <c r="H2" s="7">
-        <v>0</v>
-      </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="10" t="s">
+      <c r="C2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0</v>
+      </c>
+      <c r="I2" s="14"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="O2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="18"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="16"/>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="A3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="8">
-        <v>1</v>
-      </c>
-      <c r="G3" s="8">
-        <v>0</v>
-      </c>
-      <c r="H3" s="8">
-        <v>1</v>
-      </c>
-      <c r="I3" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8" t="s">
+      <c r="C3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <v>1</v>
+      </c>
+      <c r="I3" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="14"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" s="10" t="s">
+      <c r="K3" s="13"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="18"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="16"/>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="A4" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="7">
-        <v>1</v>
-      </c>
-      <c r="G4" s="7">
-        <v>1</v>
-      </c>
-      <c r="H4" s="7">
-        <v>0</v>
-      </c>
-      <c r="I4" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="8" t="s">
+      <c r="C4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="14"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="10" t="s">
+      <c r="K4" s="13"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="N4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="O4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="18"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="16"/>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="A5" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="7">
-        <v>1</v>
-      </c>
-      <c r="G5" s="7">
-        <v>1</v>
-      </c>
-      <c r="H5" s="7">
-        <v>1</v>
-      </c>
-      <c r="I5" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="8" t="s">
+      <c r="C5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1</v>
+      </c>
+      <c r="H5" s="6">
+        <v>1</v>
+      </c>
+      <c r="I5" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="14"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="10" t="s">
+      <c r="K5" s="13"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="N5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="O5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="18"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="16"/>
     </row>
     <row r="6" spans="1:17" s="1" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" s="7">
-        <v>1</v>
-      </c>
-      <c r="G6" s="7">
-        <v>0</v>
-      </c>
-      <c r="H6" s="7">
-        <v>0</v>
-      </c>
-      <c r="I6" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" s="8" t="s">
+      <c r="A6" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="14"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="10" t="s">
+      <c r="K6" s="13"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="N6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="O6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Selenium package update and bug fixes
1. Selenium package updates
2. Supplier name changed in release so changed logic in adding itinerary
to cart
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/Air/Air_Amadeus.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/Air/Air_Amadeus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20700" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="Air_Amadeus_OneWay" sheetId="1" r:id="rId1"/>
@@ -1838,8 +1838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1856,7 +1856,7 @@
     <col min="11" max="11" width="15.85546875" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" customWidth="1"/>
     <col min="13" max="13" width="16.140625" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" customWidth="1"/>
     <col min="15" max="15" width="11.42578125" customWidth="1"/>
     <col min="16" max="16" width="12.5703125" customWidth="1"/>
     <col min="17" max="17" width="18.5703125" customWidth="1"/>
@@ -2293,7 +2293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changes done for Hotel,Car,Activity
1. Added PreQA Transforms for Rovia and Travel Site
2. Added PreQA TestSettings for Rovia and Travel Site
3. Added references of PreQA and Stage environment into Rovia Automation
Soultion.
4. Revised Data Sheets for Air_Amadeus, Air_Sabre, Car , Hotel and
Activity
5.  Added Jquery scripts in TestHelper
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/Air/Air_Amadeus.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/Air/Air_Amadeus.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="67">
   <si>
     <t>Description</t>
   </si>
@@ -207,9 +207,6 @@
     <t>Search|setfilters|AddToCart</t>
   </si>
   <si>
-    <t>Business/Economy</t>
-  </si>
-  <si>
     <t>Search|setfilters|addtocart</t>
   </si>
   <si>
@@ -219,7 +216,7 @@
     <t>cabin</t>
   </si>
   <si>
-    <t>Search|setfilters|AddToCart|CHECKOUTTRIP|LOGIN|ENTERPAXINFO|CONFIRMPAXINFO</t>
+    <t>LOGIN|Search|AddToCart|CHECKOUTTRIP|ENTERPAXINFO|CONFIRMPAXINFO</t>
   </si>
 </sst>
 </file>
@@ -1841,9 +1838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1923,7 +1918,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>18</v>
@@ -1960,19 +1955,15 @@
       <c r="O2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q2" s="16" t="s">
-        <v>63</v>
-      </c>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="16"/>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>18</v>
@@ -2017,7 +2008,7 @@
         <v>37</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>18</v>
@@ -2062,7 +2053,7 @@
         <v>38</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>18</v>
@@ -2107,7 +2098,7 @@
         <v>39</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>18</v>
@@ -2145,7 +2136,7 @@
         <v>24</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q6" s="16"/>
     </row>
@@ -2154,7 +2145,7 @@
         <v>41</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>18</v>
@@ -2199,7 +2190,7 @@
         <v>42</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>18</v>
@@ -2244,7 +2235,7 @@
         <v>43</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C9" s="23" t="s">
         <v>18</v>
@@ -2296,8 +2287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2465,7 +2456,7 @@
         <v>24</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q3" s="16" t="s">
         <v>57</v>
@@ -2525,7 +2516,7 @@
         <v>46</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>27</v>
@@ -2574,7 +2565,7 @@
         <v>51</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>27</v>

</xml_diff>